<commit_message>
An empty project template has been created in android studio and added to this file location
</commit_message>
<xml_diff>
--- a/TM470/Planning/Gantt project planner1 _Tmplate_rename.xlsx
+++ b/TM470/Planning/Gantt project planner1 _Tmplate_rename.xlsx
@@ -2,8 +2,8 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="25831"/>
-  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{87608B1B-931B-45C9-B2FB-7DE3D20E0A23}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookPr filterPrivacy="1" codeName="ThisWorkbook" autoCompressPictures="0"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946F69DD-5F3B-4A40-A284-6B8942BDE2F3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-14300" windowWidth="21820" windowHeight="37900" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -11,14 +11,14 @@
     <sheet name="Project Planner" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="Actual">(PeriodInActual*('Project Planner'!$E1&gt;0))*PeriodInPlan</definedName>
-    <definedName name="ActualBeyond">PeriodInActual*('Project Planner'!$E1&gt;0)</definedName>
+    <definedName name="Actual">(PeriodInActual*('Project Planner'!$F1&gt;0))*PeriodInPlan</definedName>
+    <definedName name="ActualBeyond">PeriodInActual*('Project Planner'!$F1&gt;0)</definedName>
     <definedName name="PercentComplete">PercentCompleteBeyond*PeriodInPlan</definedName>
-    <definedName name="PercentCompleteBeyond">('Project Planner'!A$4=MEDIAN('Project Planner'!A$4,'Project Planner'!$E1,'Project Planner'!$E1+'Project Planner'!$F1)*('Project Planner'!$E1&gt;0))*(('Project Planner'!A$4&lt;(INT('Project Planner'!$E1+'Project Planner'!$F1*'Project Planner'!$G1)))+('Project Planner'!A$4='Project Planner'!$E1))*('Project Planner'!$G1&gt;0)</definedName>
-    <definedName name="period_selected">'Project Planner'!$H$2</definedName>
-    <definedName name="PeriodInActual">'Project Planner'!A$4=MEDIAN('Project Planner'!A$4,'Project Planner'!$E1,'Project Planner'!$E1+'Project Planner'!$F1-1)</definedName>
-    <definedName name="PeriodInPlan">'Project Planner'!A$4=MEDIAN('Project Planner'!A$4,'Project Planner'!$C1,'Project Planner'!$C1+'Project Planner'!$D1-1)</definedName>
-    <definedName name="Plan">PeriodInPlan*('Project Planner'!$C1&gt;0)</definedName>
+    <definedName name="PercentCompleteBeyond">('Project Planner'!A$4=MEDIAN('Project Planner'!A$4,'Project Planner'!$F1,'Project Planner'!$F1+'Project Planner'!$G1)*('Project Planner'!$F1&gt;0))*(('Project Planner'!A$4&lt;(INT('Project Planner'!$F1+'Project Planner'!$G1*'Project Planner'!$H1)))+('Project Planner'!A$4='Project Planner'!$F1))*('Project Planner'!$H1&gt;0)</definedName>
+    <definedName name="period_selected">'Project Planner'!$I$2</definedName>
+    <definedName name="PeriodInActual">'Project Planner'!A$4=MEDIAN('Project Planner'!A$4,'Project Planner'!$F1,'Project Planner'!$F1+'Project Planner'!$G1-1)</definedName>
+    <definedName name="PeriodInPlan">'Project Planner'!A$4=MEDIAN('Project Planner'!A$4,'Project Planner'!$D1,'Project Planner'!$D1+'Project Planner'!$E1-1)</definedName>
+    <definedName name="Plan">PeriodInPlan*('Project Planner'!$D1&gt;0)</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="0">'Project Planner'!$3:$4</definedName>
     <definedName name="TitleRegion..BO60">'Project Planner'!$B$3:$B$4</definedName>
   </definedNames>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="42" uniqueCount="42">
   <si>
     <t>Project Planner</t>
   </si>
@@ -237,6 +237,9 @@
   </si>
   <si>
     <t>Select a period to highlight at right.  A legend describing the charting follows.</t>
+  </si>
+  <si>
+    <t>SUB-TASKS          (if relevant)</t>
   </si>
 </sst>
 </file>
@@ -530,7 +533,7 @@
       <alignment horizontal="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -634,6 +637,18 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="5" applyFont="1" applyBorder="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="9" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" xfId="9" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="5" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1041,34 +1056,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <sheetPr>
+  <sheetPr codeName="Sheet1">
     <tabColor theme="7"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B1:BO30"/>
+  <dimension ref="B1:CW30"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0"/>
+    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" zoomScaleSheetLayoutView="80" workbookViewId="0">
+      <selection activeCell="H43" sqref="H43"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.77734375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="2.6640625" customWidth="1"/>
-    <col min="2" max="2" width="15.6640625" style="2" customWidth="1"/>
-    <col min="3" max="6" width="11.6640625" style="1" customWidth="1"/>
-    <col min="7" max="7" width="15.6640625" style="4" customWidth="1"/>
-    <col min="8" max="27" width="2.77734375" style="1"/>
+    <col min="2" max="3" width="15.6640625" style="2" customWidth="1"/>
+    <col min="4" max="7" width="11.6640625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="15.6640625" style="4" customWidth="1"/>
+    <col min="9" max="28" width="2.77734375" style="1"/>
+    <col min="43" max="43" width="2.77734375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:67" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.05">
+    <row r="1" spans="2:101" ht="60" customHeight="1" thickBot="1" x14ac:dyDescent="1.05">
       <c r="B1" s="14" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="13"/>
+      <c r="C1" s="14"/>
       <c r="D1" s="13"/>
       <c r="E1" s="13"/>
       <c r="F1" s="13"/>
       <c r="G1" s="13"/>
-    </row>
-    <row r="2" spans="2:67" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="H1" s="13"/>
+    </row>
+    <row r="2" spans="2:101" ht="21" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B2" s="22" t="s">
         <v>40</v>
       </c>
@@ -1076,80 +1095,83 @@
       <c r="D2" s="22"/>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
-      <c r="G2" s="5" t="s">
+      <c r="G2" s="22"/>
+      <c r="H2" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H2" s="15">
-        <v>1</v>
-      </c>
-      <c r="J2" s="16"/>
-      <c r="K2" s="30" t="s">
+      <c r="I2" s="15">
+        <v>60</v>
+      </c>
+      <c r="K2" s="16"/>
+      <c r="L2" s="30" t="s">
         <v>39</v>
       </c>
-      <c r="L2" s="31"/>
       <c r="M2" s="31"/>
       <c r="N2" s="31"/>
-      <c r="O2" s="32"/>
-      <c r="P2" s="17"/>
-      <c r="Q2" s="30" t="s">
+      <c r="O2" s="31"/>
+      <c r="P2" s="32"/>
+      <c r="Q2" s="17"/>
+      <c r="R2" s="30" t="s">
         <v>38</v>
       </c>
-      <c r="R2" s="33"/>
       <c r="S2" s="33"/>
-      <c r="T2" s="32"/>
-      <c r="U2" s="18"/>
-      <c r="V2" s="23" t="s">
+      <c r="T2" s="33"/>
+      <c r="U2" s="32"/>
+      <c r="V2" s="18"/>
+      <c r="W2" s="23" t="s">
         <v>29</v>
       </c>
-      <c r="W2" s="24"/>
       <c r="X2" s="24"/>
-      <c r="Y2" s="34"/>
-      <c r="Z2" s="19"/>
-      <c r="AA2" s="23" t="s">
+      <c r="Y2" s="24"/>
+      <c r="Z2" s="34"/>
+      <c r="AA2" s="19"/>
+      <c r="AB2" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="AB2" s="24"/>
       <c r="AC2" s="24"/>
       <c r="AD2" s="24"/>
       <c r="AE2" s="24"/>
       <c r="AF2" s="24"/>
-      <c r="AG2" s="34"/>
-      <c r="AH2" s="20"/>
-      <c r="AI2" s="23" t="s">
+      <c r="AG2" s="24"/>
+      <c r="AH2" s="34"/>
+      <c r="AI2" s="20"/>
+      <c r="AJ2" s="37" t="s">
         <v>31</v>
       </c>
-      <c r="AJ2" s="24"/>
-      <c r="AK2" s="24"/>
-      <c r="AL2" s="24"/>
-      <c r="AM2" s="24"/>
-      <c r="AN2" s="24"/>
-      <c r="AO2" s="24"/>
-      <c r="AP2" s="24"/>
-    </row>
-    <row r="3" spans="2:67" s="12" customFormat="1" ht="39.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
+      <c r="AK2" s="38"/>
+      <c r="AL2" s="38"/>
+      <c r="AM2" s="38"/>
+      <c r="AN2" s="38"/>
+      <c r="AO2" s="38"/>
+      <c r="AP2" s="38"/>
+      <c r="AQ2" s="38"/>
+    </row>
+    <row r="3" spans="2:101" s="12" customFormat="1" ht="39.9" customHeight="1" thickTop="1" x14ac:dyDescent="0.3">
       <c r="B3" s="25" t="s">
         <v>2</v>
       </c>
-      <c r="C3" s="27" t="s">
+      <c r="C3" s="35" t="s">
+        <v>41</v>
+      </c>
+      <c r="D3" s="27" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="27" t="s">
+      <c r="E3" s="27" t="s">
         <v>34</v>
       </c>
-      <c r="E3" s="27" t="s">
+      <c r="F3" s="27" t="s">
         <v>35</v>
       </c>
-      <c r="F3" s="27" t="s">
+      <c r="G3" s="27" t="s">
         <v>36</v>
       </c>
-      <c r="G3" s="29" t="s">
+      <c r="H3" s="29" t="s">
         <v>37</v>
       </c>
-      <c r="H3" s="21" t="s">
+      <c r="I3" s="21" t="s">
         <v>1</v>
       </c>
-      <c r="I3" s="10"/>
-      <c r="J3" s="11"/>
+      <c r="J3" s="10"/>
       <c r="K3" s="11"/>
       <c r="L3" s="11"/>
       <c r="M3" s="11"/>
@@ -1167,730 +1189,858 @@
       <c r="Y3" s="11"/>
       <c r="Z3" s="11"/>
       <c r="AA3" s="11"/>
-    </row>
-    <row r="4" spans="2:67" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="AB3" s="11"/>
+    </row>
+    <row r="4" spans="2:101" ht="15.75" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B4" s="26"/>
-      <c r="C4" s="28"/>
+      <c r="C4" s="36"/>
       <c r="D4" s="28"/>
       <c r="E4" s="28"/>
       <c r="F4" s="28"/>
       <c r="G4" s="28"/>
-      <c r="H4" s="3">
+      <c r="H4" s="28"/>
+      <c r="I4" s="3">
         <v>1</v>
       </c>
-      <c r="I4" s="3">
+      <c r="J4" s="3">
         <v>2</v>
       </c>
-      <c r="J4" s="3">
+      <c r="K4" s="3">
         <v>3</v>
       </c>
-      <c r="K4" s="3">
+      <c r="L4" s="3">
         <v>4</v>
       </c>
-      <c r="L4" s="3">
+      <c r="M4" s="3">
         <v>5</v>
       </c>
-      <c r="M4" s="3">
+      <c r="N4" s="3">
         <v>6</v>
       </c>
-      <c r="N4" s="3">
+      <c r="O4" s="3">
         <v>7</v>
       </c>
-      <c r="O4" s="3">
+      <c r="P4" s="3">
         <v>8</v>
       </c>
-      <c r="P4" s="3">
+      <c r="Q4" s="3">
         <v>9</v>
       </c>
-      <c r="Q4" s="3">
+      <c r="R4" s="3">
         <v>10</v>
       </c>
-      <c r="R4" s="3">
+      <c r="S4" s="3">
         <v>11</v>
       </c>
-      <c r="S4" s="3">
+      <c r="T4" s="3">
         <v>12</v>
       </c>
-      <c r="T4" s="3">
+      <c r="U4" s="3">
         <v>13</v>
       </c>
-      <c r="U4" s="3">
+      <c r="V4" s="3">
         <v>14</v>
       </c>
-      <c r="V4" s="3">
+      <c r="W4" s="3">
         <v>15</v>
       </c>
-      <c r="W4" s="3">
+      <c r="X4" s="3">
         <v>16</v>
       </c>
-      <c r="X4" s="3">
+      <c r="Y4" s="3">
         <v>17</v>
       </c>
-      <c r="Y4" s="3">
+      <c r="Z4" s="3">
         <v>18</v>
       </c>
-      <c r="Z4" s="3">
+      <c r="AA4" s="3">
         <v>19</v>
       </c>
-      <c r="AA4" s="3">
+      <c r="AB4" s="3">
         <v>20</v>
       </c>
-      <c r="AB4" s="3">
+      <c r="AC4" s="3">
         <v>21</v>
       </c>
-      <c r="AC4" s="3">
+      <c r="AD4" s="3">
         <v>22</v>
       </c>
-      <c r="AD4" s="3">
+      <c r="AE4" s="3">
         <v>23</v>
       </c>
-      <c r="AE4" s="3">
+      <c r="AF4" s="3">
         <v>24</v>
       </c>
-      <c r="AF4" s="3">
+      <c r="AG4" s="3">
         <v>25</v>
       </c>
-      <c r="AG4" s="3">
+      <c r="AH4" s="3">
         <v>26</v>
       </c>
-      <c r="AH4" s="3">
+      <c r="AI4" s="3">
         <v>27</v>
       </c>
-      <c r="AI4" s="3">
+      <c r="AJ4" s="3">
         <v>28</v>
       </c>
-      <c r="AJ4" s="3">
+      <c r="AK4" s="3">
         <v>29</v>
       </c>
-      <c r="AK4" s="3">
+      <c r="AL4" s="3">
         <v>30</v>
       </c>
-      <c r="AL4" s="3">
+      <c r="AM4" s="3">
         <v>31</v>
       </c>
-      <c r="AM4" s="3">
+      <c r="AN4" s="3">
         <v>32</v>
       </c>
-      <c r="AN4" s="3">
+      <c r="AO4" s="3">
         <v>33</v>
       </c>
-      <c r="AO4" s="3">
+      <c r="AP4" s="3">
         <v>34</v>
       </c>
-      <c r="AP4" s="3">
+      <c r="AQ4" s="3">
         <v>35</v>
       </c>
-      <c r="AQ4" s="3">
+      <c r="AR4" s="3">
         <v>36</v>
       </c>
-      <c r="AR4" s="3">
+      <c r="AS4" s="3">
         <v>37</v>
       </c>
-      <c r="AS4" s="3">
+      <c r="AT4" s="3">
         <v>38</v>
       </c>
-      <c r="AT4" s="3">
+      <c r="AU4" s="3">
         <v>39</v>
       </c>
-      <c r="AU4" s="3">
+      <c r="AV4" s="3">
         <v>40</v>
       </c>
-      <c r="AV4" s="3">
+      <c r="AW4" s="3">
         <v>41</v>
       </c>
-      <c r="AW4" s="3">
+      <c r="AX4" s="3">
         <v>42</v>
       </c>
-      <c r="AX4" s="3">
+      <c r="AY4" s="3">
         <v>43</v>
       </c>
-      <c r="AY4" s="3">
+      <c r="AZ4" s="3">
         <v>44</v>
       </c>
-      <c r="AZ4" s="3">
+      <c r="BA4" s="3">
         <v>45</v>
       </c>
-      <c r="BA4" s="3">
+      <c r="BB4" s="3">
         <v>46</v>
       </c>
-      <c r="BB4" s="3">
+      <c r="BC4" s="3">
         <v>47</v>
       </c>
-      <c r="BC4" s="3">
+      <c r="BD4" s="3">
         <v>48</v>
       </c>
-      <c r="BD4" s="3">
+      <c r="BE4" s="3">
         <v>49</v>
       </c>
-      <c r="BE4" s="3">
+      <c r="BF4" s="3">
         <v>50</v>
       </c>
-      <c r="BF4" s="3">
+      <c r="BG4" s="3">
         <v>51</v>
       </c>
-      <c r="BG4" s="3">
+      <c r="BH4" s="3">
         <v>52</v>
       </c>
-      <c r="BH4" s="3">
+      <c r="BI4" s="3">
         <v>53</v>
       </c>
-      <c r="BI4" s="3">
+      <c r="BJ4" s="3">
         <v>54</v>
       </c>
-      <c r="BJ4" s="3">
+      <c r="BK4" s="3">
         <v>55</v>
       </c>
-      <c r="BK4" s="3">
+      <c r="BL4" s="3">
         <v>56</v>
       </c>
-      <c r="BL4" s="3">
+      <c r="BM4" s="3">
         <v>57</v>
       </c>
-      <c r="BM4" s="3">
+      <c r="BN4" s="3">
         <v>58</v>
       </c>
-      <c r="BN4" s="3">
+      <c r="BO4" s="3">
         <v>59</v>
       </c>
-      <c r="BO4" s="3">
+      <c r="BP4" s="3">
         <v>60</v>
       </c>
-    </row>
-    <row r="5" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="BQ4" s="3">
+        <v>61</v>
+      </c>
+      <c r="BR4" s="3">
+        <v>62</v>
+      </c>
+      <c r="BS4" s="3">
+        <v>63</v>
+      </c>
+      <c r="BT4" s="3">
+        <v>64</v>
+      </c>
+      <c r="BU4" s="3">
+        <v>65</v>
+      </c>
+      <c r="BV4" s="3">
+        <v>66</v>
+      </c>
+      <c r="BW4" s="3">
+        <v>67</v>
+      </c>
+      <c r="BX4" s="3">
+        <v>68</v>
+      </c>
+      <c r="BY4" s="3">
+        <v>69</v>
+      </c>
+      <c r="BZ4" s="3">
+        <v>70</v>
+      </c>
+      <c r="CA4" s="3">
+        <v>71</v>
+      </c>
+      <c r="CB4" s="3">
+        <v>72</v>
+      </c>
+      <c r="CC4" s="3">
+        <v>73</v>
+      </c>
+      <c r="CD4" s="3">
+        <v>74</v>
+      </c>
+      <c r="CE4" s="3">
+        <v>75</v>
+      </c>
+      <c r="CF4" s="3">
+        <v>76</v>
+      </c>
+      <c r="CG4" s="3">
+        <v>77</v>
+      </c>
+      <c r="CH4" s="3">
+        <v>78</v>
+      </c>
+      <c r="CI4" s="3">
+        <v>79</v>
+      </c>
+      <c r="CJ4" s="3">
+        <v>80</v>
+      </c>
+      <c r="CK4" s="3">
+        <v>81</v>
+      </c>
+      <c r="CL4" s="3">
+        <v>82</v>
+      </c>
+      <c r="CM4" s="3">
+        <v>83</v>
+      </c>
+      <c r="CN4" s="3">
+        <v>84</v>
+      </c>
+      <c r="CO4" s="3">
+        <v>85</v>
+      </c>
+      <c r="CP4" s="3">
+        <v>86</v>
+      </c>
+      <c r="CQ4" s="3">
+        <v>87</v>
+      </c>
+      <c r="CR4" s="3">
+        <v>88</v>
+      </c>
+      <c r="CS4" s="3">
+        <v>89</v>
+      </c>
+      <c r="CT4" s="3">
+        <v>90</v>
+      </c>
+      <c r="CU4" s="3">
+        <v>91</v>
+      </c>
+      <c r="CV4" s="3">
+        <v>92</v>
+      </c>
+      <c r="CW4" s="3">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="5" spans="2:101" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="6" t="s">
         <v>3</v>
       </c>
-      <c r="C5" s="7">
+      <c r="C5" s="6"/>
+      <c r="D5" s="7">
         <v>1</v>
       </c>
-      <c r="D5" s="7">
+      <c r="E5" s="7">
         <v>5</v>
       </c>
-      <c r="E5" s="7">
+      <c r="F5" s="7">
         <v>1</v>
       </c>
-      <c r="F5" s="7">
+      <c r="G5" s="7">
         <v>4</v>
       </c>
-      <c r="G5" s="8">
+      <c r="H5" s="8">
         <v>0.25</v>
       </c>
     </row>
-    <row r="6" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:101" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B6" s="6" t="s">
         <v>4</v>
       </c>
-      <c r="C6" s="7">
+      <c r="C6" s="6"/>
+      <c r="D6" s="7">
         <v>1</v>
       </c>
-      <c r="D6" s="7">
+      <c r="E6" s="7">
         <v>6</v>
       </c>
-      <c r="E6" s="7">
+      <c r="F6" s="7">
         <v>1</v>
       </c>
-      <c r="F6" s="7">
+      <c r="G6" s="7">
         <v>6</v>
       </c>
-      <c r="G6" s="8">
+      <c r="H6" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:101" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B7" s="6" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="7">
+      <c r="C7" s="6"/>
+      <c r="D7" s="7">
         <v>2</v>
       </c>
-      <c r="D7" s="7">
+      <c r="E7" s="7">
         <v>4</v>
       </c>
-      <c r="E7" s="7">
+      <c r="F7" s="7">
         <v>2</v>
       </c>
-      <c r="F7" s="7">
+      <c r="G7" s="7">
         <v>5</v>
       </c>
-      <c r="G7" s="8">
+      <c r="H7" s="8">
         <v>0.35</v>
       </c>
     </row>
-    <row r="8" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:101" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B8" s="6" t="s">
         <v>6</v>
       </c>
-      <c r="C8" s="7">
+      <c r="C8" s="6"/>
+      <c r="D8" s="7">
         <v>4</v>
       </c>
-      <c r="D8" s="7">
+      <c r="E8" s="7">
         <v>8</v>
       </c>
-      <c r="E8" s="7">
+      <c r="F8" s="7">
         <v>4</v>
       </c>
-      <c r="F8" s="7">
+      <c r="G8" s="7">
         <v>6</v>
       </c>
-      <c r="G8" s="8">
+      <c r="H8" s="8">
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:101" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B9" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="C9" s="7">
+      <c r="C9" s="6"/>
+      <c r="D9" s="7">
         <v>4</v>
       </c>
-      <c r="D9" s="7">
+      <c r="E9" s="7">
         <v>2</v>
       </c>
-      <c r="E9" s="7">
+      <c r="F9" s="7">
         <v>4</v>
       </c>
-      <c r="F9" s="7">
+      <c r="G9" s="7">
         <v>8</v>
       </c>
-      <c r="G9" s="8">
+      <c r="H9" s="8">
         <v>0.85</v>
       </c>
     </row>
-    <row r="10" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:101" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B10" s="6" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="7">
+      <c r="C10" s="6"/>
+      <c r="D10" s="7">
         <v>4</v>
       </c>
-      <c r="D10" s="7">
+      <c r="E10" s="7">
         <v>3</v>
       </c>
-      <c r="E10" s="7">
+      <c r="F10" s="7">
         <v>4</v>
       </c>
-      <c r="F10" s="7">
+      <c r="G10" s="7">
         <v>6</v>
       </c>
-      <c r="G10" s="8">
+      <c r="H10" s="8">
         <v>0.85</v>
       </c>
     </row>
-    <row r="11" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:101" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B11" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="7">
+      <c r="C11" s="6"/>
+      <c r="D11" s="7">
         <v>5</v>
       </c>
-      <c r="D11" s="7">
+      <c r="E11" s="7">
         <v>4</v>
       </c>
-      <c r="E11" s="7">
+      <c r="F11" s="7">
         <v>5</v>
       </c>
-      <c r="F11" s="7">
+      <c r="G11" s="7">
         <v>3</v>
       </c>
-      <c r="G11" s="8">
+      <c r="H11" s="8">
         <v>0.5</v>
       </c>
     </row>
-    <row r="12" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:101" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B12" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="C12" s="7">
+      <c r="C12" s="6"/>
+      <c r="D12" s="7">
         <v>5</v>
       </c>
-      <c r="D12" s="7">
+      <c r="E12" s="7">
         <v>2</v>
-      </c>
-      <c r="E12" s="7">
-        <v>5</v>
       </c>
       <c r="F12" s="7">
         <v>5</v>
       </c>
-      <c r="G12" s="8">
+      <c r="G12" s="7">
+        <v>5</v>
+      </c>
+      <c r="H12" s="8">
         <v>0.6</v>
       </c>
     </row>
-    <row r="13" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="13" spans="2:101" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B13" s="6" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="7">
+      <c r="C13" s="6"/>
+      <c r="D13" s="7">
         <v>5</v>
       </c>
-      <c r="D13" s="7">
+      <c r="E13" s="7">
         <v>2</v>
       </c>
-      <c r="E13" s="7">
+      <c r="F13" s="7">
         <v>5</v>
       </c>
-      <c r="F13" s="7">
+      <c r="G13" s="7">
         <v>6</v>
       </c>
-      <c r="G13" s="8">
+      <c r="H13" s="8">
         <v>0.75</v>
       </c>
     </row>
-    <row r="14" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:101" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B14" s="6" t="s">
         <v>12</v>
       </c>
-      <c r="C14" s="7">
+      <c r="C14" s="6"/>
+      <c r="D14" s="7">
         <v>6</v>
       </c>
-      <c r="D14" s="7">
+      <c r="E14" s="7">
         <v>5</v>
       </c>
-      <c r="E14" s="7">
+      <c r="F14" s="7">
         <v>6</v>
       </c>
-      <c r="F14" s="7">
+      <c r="G14" s="7">
         <v>7</v>
       </c>
-      <c r="G14" s="8">
+      <c r="H14" s="8">
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:101" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6" t="s">
         <v>13</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="6"/>
+      <c r="D15" s="9">
         <v>6</v>
       </c>
-      <c r="D15" s="7">
+      <c r="E15" s="7">
         <v>1</v>
       </c>
-      <c r="E15" s="7">
+      <c r="F15" s="7">
         <v>5</v>
       </c>
-      <c r="F15" s="7">
+      <c r="G15" s="7">
         <v>8</v>
       </c>
-      <c r="G15" s="8">
+      <c r="H15" s="8">
         <v>0.6</v>
       </c>
     </row>
-    <row r="16" spans="2:67" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:101" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B16" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="C16" s="7">
+      <c r="C16" s="6"/>
+      <c r="D16" s="7">
         <v>9</v>
       </c>
-      <c r="D16" s="7">
+      <c r="E16" s="7">
         <v>3</v>
       </c>
-      <c r="E16" s="7">
+      <c r="F16" s="7">
         <v>9</v>
       </c>
-      <c r="F16" s="7">
+      <c r="G16" s="7">
         <v>3</v>
       </c>
-      <c r="G16" s="8">
+      <c r="H16" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B17" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="C17" s="7">
+      <c r="C17" s="6"/>
+      <c r="D17" s="7">
         <v>9</v>
       </c>
-      <c r="D17" s="7">
+      <c r="E17" s="7">
         <v>6</v>
       </c>
-      <c r="E17" s="7">
+      <c r="F17" s="7">
         <v>9</v>
       </c>
-      <c r="F17" s="7">
+      <c r="G17" s="7">
         <v>7</v>
       </c>
-      <c r="G17" s="8">
+      <c r="H17" s="8">
         <v>0.5</v>
       </c>
     </row>
-    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B18" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="C18" s="7">
+      <c r="C18" s="6"/>
+      <c r="D18" s="7">
         <v>9</v>
       </c>
-      <c r="D18" s="7">
+      <c r="E18" s="7">
         <v>3</v>
       </c>
-      <c r="E18" s="7">
+      <c r="F18" s="7">
         <v>9</v>
       </c>
-      <c r="F18" s="7">
+      <c r="G18" s="7">
         <v>1</v>
       </c>
-      <c r="G18" s="8">
+      <c r="H18" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B19" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="C19" s="7">
+      <c r="C19" s="6"/>
+      <c r="D19" s="7">
         <v>9</v>
       </c>
-      <c r="D19" s="7">
+      <c r="E19" s="7">
         <v>4</v>
       </c>
-      <c r="E19" s="7">
+      <c r="F19" s="7">
         <v>8</v>
       </c>
-      <c r="F19" s="7">
+      <c r="G19" s="7">
         <v>5</v>
       </c>
-      <c r="G19" s="8">
+      <c r="H19" s="8">
         <v>0.01</v>
       </c>
     </row>
-    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B20" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="C20" s="7">
+      <c r="C20" s="6"/>
+      <c r="D20" s="7">
         <v>10</v>
       </c>
-      <c r="D20" s="7">
+      <c r="E20" s="7">
         <v>5</v>
       </c>
-      <c r="E20" s="7">
+      <c r="F20" s="7">
         <v>10</v>
       </c>
-      <c r="F20" s="7">
+      <c r="G20" s="7">
         <v>3</v>
       </c>
-      <c r="G20" s="8">
+      <c r="H20" s="8">
         <v>0.8</v>
       </c>
     </row>
-    <row r="21" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="21" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B21" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C21" s="7">
+      <c r="C21" s="6"/>
+      <c r="D21" s="7">
         <v>11</v>
       </c>
-      <c r="D21" s="7">
+      <c r="E21" s="7">
         <v>2</v>
       </c>
-      <c r="E21" s="7">
+      <c r="F21" s="7">
         <v>11</v>
       </c>
-      <c r="F21" s="7">
+      <c r="G21" s="7">
         <v>5</v>
       </c>
-      <c r="G21" s="8">
+      <c r="H21" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B22" s="6" t="s">
         <v>20</v>
       </c>
-      <c r="C22" s="7">
+      <c r="C22" s="6"/>
+      <c r="D22" s="7">
         <v>12</v>
       </c>
-      <c r="D22" s="7">
+      <c r="E22" s="7">
         <v>6</v>
       </c>
-      <c r="E22" s="7">
+      <c r="F22" s="7">
         <v>12</v>
       </c>
-      <c r="F22" s="7">
+      <c r="G22" s="7">
         <v>7</v>
       </c>
-      <c r="G22" s="8">
+      <c r="H22" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B23" s="6" t="s">
         <v>21</v>
       </c>
-      <c r="C23" s="7">
+      <c r="C23" s="6"/>
+      <c r="D23" s="7">
         <v>12</v>
       </c>
-      <c r="D23" s="7">
+      <c r="E23" s="7">
         <v>1</v>
       </c>
-      <c r="E23" s="7">
+      <c r="F23" s="7">
         <v>12</v>
       </c>
-      <c r="F23" s="7">
+      <c r="G23" s="7">
         <v>5</v>
       </c>
-      <c r="G23" s="8">
+      <c r="H23" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B24" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="7">
+      <c r="C24" s="6"/>
+      <c r="D24" s="7">
         <v>14</v>
       </c>
-      <c r="D24" s="7">
+      <c r="E24" s="7">
         <v>5</v>
       </c>
-      <c r="E24" s="7">
+      <c r="F24" s="7">
         <v>14</v>
       </c>
-      <c r="F24" s="7">
+      <c r="G24" s="7">
         <v>6</v>
       </c>
-      <c r="G24" s="8">
+      <c r="H24" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B25" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="C25" s="7">
+      <c r="C25" s="6"/>
+      <c r="D25" s="7">
         <v>14</v>
       </c>
-      <c r="D25" s="7">
+      <c r="E25" s="7">
         <v>8</v>
       </c>
-      <c r="E25" s="7">
+      <c r="F25" s="7">
         <v>14</v>
       </c>
-      <c r="F25" s="7">
+      <c r="G25" s="7">
         <v>2</v>
       </c>
-      <c r="G25" s="8">
+      <c r="H25" s="8">
         <v>0.44</v>
       </c>
     </row>
-    <row r="26" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B26" s="6" t="s">
         <v>24</v>
       </c>
-      <c r="C26" s="7">
+      <c r="C26" s="6"/>
+      <c r="D26" s="7">
         <v>14</v>
       </c>
-      <c r="D26" s="7">
+      <c r="E26" s="7">
         <v>7</v>
       </c>
-      <c r="E26" s="7">
+      <c r="F26" s="7">
         <v>14</v>
       </c>
-      <c r="F26" s="7">
+      <c r="G26" s="7">
         <v>3</v>
       </c>
-      <c r="G26" s="8">
+      <c r="H26" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B27" s="6" t="s">
         <v>25</v>
       </c>
-      <c r="C27" s="7">
+      <c r="C27" s="6"/>
+      <c r="D27" s="7">
         <v>15</v>
       </c>
-      <c r="D27" s="7">
+      <c r="E27" s="7">
         <v>4</v>
       </c>
-      <c r="E27" s="7">
+      <c r="F27" s="7">
         <v>15</v>
       </c>
-      <c r="F27" s="7">
+      <c r="G27" s="7">
         <v>8</v>
       </c>
-      <c r="G27" s="8">
+      <c r="H27" s="8">
         <v>0.12</v>
       </c>
     </row>
-    <row r="28" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B28" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="C28" s="7">
+      <c r="C28" s="6"/>
+      <c r="D28" s="7">
         <v>15</v>
       </c>
-      <c r="D28" s="7">
+      <c r="E28" s="7">
         <v>5</v>
       </c>
-      <c r="E28" s="7">
+      <c r="F28" s="7">
         <v>15</v>
       </c>
-      <c r="F28" s="7">
+      <c r="G28" s="7">
         <v>3</v>
       </c>
-      <c r="G28" s="8">
+      <c r="H28" s="8">
         <v>0.05</v>
       </c>
     </row>
-    <row r="29" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B29" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="C29" s="7">
+      <c r="C29" s="6"/>
+      <c r="D29" s="7">
         <v>15</v>
       </c>
-      <c r="D29" s="7">
+      <c r="E29" s="7">
         <v>8</v>
       </c>
-      <c r="E29" s="7">
+      <c r="F29" s="7">
         <v>15</v>
       </c>
-      <c r="F29" s="7">
+      <c r="G29" s="7">
         <v>5</v>
       </c>
-      <c r="G29" s="8">
+      <c r="H29" s="8">
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B30" s="6" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="7">
+      <c r="C30" s="6"/>
+      <c r="D30" s="7">
         <v>16</v>
       </c>
-      <c r="D30" s="7">
+      <c r="E30" s="7">
         <v>28</v>
       </c>
-      <c r="E30" s="7">
+      <c r="F30" s="7">
         <v>16</v>
       </c>
-      <c r="F30" s="7">
+      <c r="G30" s="7">
         <v>30</v>
       </c>
-      <c r="G30" s="8">
+      <c r="H30" s="8">
         <v>0.5</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="AI2:AP2"/>
+  <mergeCells count="12">
+    <mergeCell ref="AJ2:AQ2"/>
     <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
     <mergeCell ref="D3:D4"/>
     <mergeCell ref="E3:E4"/>
     <mergeCell ref="F3:F4"/>
     <mergeCell ref="G3:G4"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="Q2:T2"/>
-    <mergeCell ref="V2:Y2"/>
-    <mergeCell ref="AA2:AG2"/>
+    <mergeCell ref="H3:H4"/>
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="R2:U2"/>
+    <mergeCell ref="W2:Z2"/>
+    <mergeCell ref="AB2:AH2"/>
+    <mergeCell ref="C3:C4"/>
   </mergeCells>
-  <conditionalFormatting sqref="H5:BO30">
+  <conditionalFormatting sqref="I5:CW30">
     <cfRule type="expression" dxfId="9" priority="1">
       <formula>PercentComplete</formula>
     </cfRule>
@@ -1907,7 +2057,7 @@
       <formula>Plan</formula>
     </cfRule>
     <cfRule type="expression" dxfId="4" priority="7">
-      <formula>H$4=period_selected</formula>
+      <formula>I$4=period_selected</formula>
     </cfRule>
     <cfRule type="expression" dxfId="3" priority="11">
       <formula>MOD(COLUMN(),2)</formula>
@@ -1916,42 +2066,40 @@
       <formula>MOD(COLUMN(),2)=0</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B31:BO31">
+  <conditionalFormatting sqref="B31:BP31">
     <cfRule type="expression" dxfId="1" priority="2">
       <formula>TRUE</formula>
     </cfRule>
   </conditionalFormatting>
-  <conditionalFormatting sqref="H4:BO4">
+  <conditionalFormatting sqref="I4:CW4">
     <cfRule type="expression" dxfId="0" priority="8">
-      <formula>H$4=period_selected</formula>
+      <formula>I$4=period_selected</formula>
     </cfRule>
   </conditionalFormatting>
   <dataValidations count="16">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Project planner uses periods for intervals. Start=1 is period 1 and duration=5 means project spans 5 periods starting from start period. Enter data starting in B5 to update the chart" sqref="A1" xr:uid="{00000000-0002-0000-0000-000000000000}"/>
-    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Type a value from 1 to 60 or select a period from the list-press  CANCEL, ALT+DOWN ARROW, then ENTER to select a value" prompt="Enter a period in the range of 1 to 60 or select a period from the list. Press ALT+DOWN ARROW to navigate the list, then ENTER to select a value" sqref="H2" xr:uid="{00000000-0002-0000-0000-000001000000}">
+    <dataValidation type="list" errorStyle="warning" allowBlank="1" showInputMessage="1" showErrorMessage="1" error="Type a value from 1 to 60 or select a period from the list-press  CANCEL, ALT+DOWN ARROW, then ENTER to select a value" prompt="Enter a period in the range of 1 to 60 or select a period from the list. Press ALT+DOWN ARROW to navigate the list, then ENTER to select a value" sqref="I2" xr:uid="{00000000-0002-0000-0000-000001000000}">
       <formula1>"1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50,51,52,53,54,55,56,57,58,59,60"</formula1>
     </dataValidation>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates plan duration" sqref="J2" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration" sqref="P2" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed" sqref="U2" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration beyond plan" sqref="Z2" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed beyond plan" sqref="AH2" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Periods are charted from 1 to 60 starting from cell H4 to cell BO4 " sqref="H3" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter activity in column B, starting with cell B5_x000a_" sqref="B3:B4" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan start period in column C, starting with cell C5" sqref="C3:C4" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan duration period in column D, starting with cell D5" sqref="D3:D4" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual start period in column E, starting with cell E5" sqref="E3:E4" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual duration period in column F, starting with cell F5" sqref="F3:F4" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the percentage of project completed in column G, starting with cell G5" sqref="G3:G4" xr:uid="{00000000-0002-0000-0000-00000D000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of the project. Enter a new title in this cell. Highlight a period in H2. Chart legend is in J2 to AI2" sqref="B1" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select a period to highlight in H2. A Chart legend is in J2 to AI2" sqref="B2:F2" xr:uid="{00000000-0002-0000-0000-00000F000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates plan duration" sqref="K2" xr:uid="{00000000-0002-0000-0000-000002000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration" sqref="Q2" xr:uid="{00000000-0002-0000-0000-000003000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed" sqref="V2" xr:uid="{00000000-0002-0000-0000-000004000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates actual duration beyond plan" sqref="AA2" xr:uid="{00000000-0002-0000-0000-000005000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="This legend cell indicates the percentage of project completed beyond plan" sqref="AI2" xr:uid="{00000000-0002-0000-0000-000006000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Periods are charted from 1 to 60 starting from cell H4 to cell BO4 " sqref="I3" xr:uid="{00000000-0002-0000-0000-000007000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter activity in column B, starting with cell B5_x000a_" sqref="B3:B4 C3" xr:uid="{00000000-0002-0000-0000-000008000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan start period in column C, starting with cell C5" sqref="D3:D4" xr:uid="{00000000-0002-0000-0000-000009000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter plan duration period in column D, starting with cell D5" sqref="E3:E4" xr:uid="{00000000-0002-0000-0000-00000A000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual start period in column E, starting with cell E5" sqref="F3:F4" xr:uid="{00000000-0002-0000-0000-00000B000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter actual duration period in column F, starting with cell F5" sqref="G3:G4" xr:uid="{00000000-0002-0000-0000-00000C000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Enter the percentage of project completed in column G, starting with cell G5" sqref="H3:H4" xr:uid="{00000000-0002-0000-0000-00000D000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Title of the project. Enter a new title in this cell. Highlight a period in H2. Chart legend is in J2 to AI2" sqref="B1:C1" xr:uid="{00000000-0002-0000-0000-00000E000000}"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" prompt="Select a period to highlight in H2. A Chart legend is in J2 to AI2" sqref="B2:G2" xr:uid="{00000000-0002-0000-0000-00000F000000}"/>
   </dataValidations>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0.45" right="0.45" top="0.5" bottom="0.5" header="0.3" footer="0.3"/>
-  <pageSetup scale="51" fitToHeight="0" orientation="landscape" r:id="rId1"/>
-  <headerFooter differentFirst="1">
-    <oddFooter>Page &amp;P of &amp;N</oddFooter>
-  </headerFooter>
+  <pageSetup scale="35" fitToHeight="0" orientation="landscape" r:id="rId1"/>
+  <headerFooter differentFirst="1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
       <mx:PLV Mode="0" OnePage="0" WScale="0"/>

</xml_diff>